<commit_message>
HospitalData 엑셀 수정 / HospitalExcel class 실행 시 널포인터 오류 해결
</commit_message>
<xml_diff>
--- a/data/HospitalData.xlsx
+++ b/data/HospitalData.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3949747-CCA6-4E81-AA92-39A9CB0FBA0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="병원정보" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
   <si>
     <t>시/구</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -45,10 +46,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>연세대 세브란스병원</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>경기도 고양시</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -61,10 +58,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>부산 해운대구</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>해운대로 875</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -89,18 +82,190 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>방어진동 535</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>울산대학교 병원</t>
+    <t>신촌세브란스병원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대사관로 59</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>순천향대학교서울병원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>반포대로 222 가톨릭중앙의료원 새병원 및 성의회관</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가톨릭대학교 서울성모병원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울특별시 용산구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울특별시 서초구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울특별시 은평구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>진흥로 191</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울병원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울특별시 강동구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>양재대로 1525</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>올바른서울병원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>남부순환로 2584</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서초보건소</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>경기도 안양시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>동안구 시민대로 388</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>평촌 서울나우병원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울특별시 강남구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일원로 81 삼성의료원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>삼성서울병원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>경기도 성남시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>분당구 구미로 173번길 82</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>분당서울대학교병원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부산광역시 남구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>용호로 232번길 25-14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부산성모병원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부산광역시 해운대구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부산광역시 서구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대신공원로 26</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>동아대학교병원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부산광역시 북구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>금곡대로 348</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부산북구보건소</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>방어진순환도로 877</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>울산대학교병원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>경기도 파주시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>후곡로 13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파주시 보건소</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울특별시 마포구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>월드컵로 212</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마포보건소</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울특별시 성동구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>왕십리로 222-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한양대학교병원</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -154,6 +319,19 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2257088D-026F-4726-8A0E-D1E193A0E4F6}" name="표1" displayName="표1" ref="A1:D20" totalsRowShown="0">
+  <autoFilter ref="A1:D20" xr:uid="{2257088D-026F-4726-8A0E-D1E193A0E4F6}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{58053CDF-7813-445E-AFAF-0CD80F600EF3}" name="시/구"/>
+    <tableColumn id="2" xr3:uid="{99E354D6-71F2-48ED-804A-42A051B81F7A}" name="상세주소"/>
+    <tableColumn id="3" xr3:uid="{60A882C8-076B-41CE-8BFE-BC098A13704E}" name="병원명"/>
+    <tableColumn id="4" xr3:uid="{9625496F-80FF-4474-BC1C-45A967C63A2C}" name="백신재고수량"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -418,17 +596,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30.625" customWidth="1"/>
-    <col min="2" max="3" width="40.625" customWidth="1"/>
+    <col min="2" max="2" width="50.625" customWidth="1"/>
+    <col min="3" max="3" width="40.625" customWidth="1"/>
     <col min="4" max="4" width="20.625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -454,7 +633,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D2">
         <v>150</v>
@@ -462,13 +641,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
       </c>
       <c r="D3">
         <v>128</v>
@@ -476,13 +655,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
         <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
       </c>
       <c r="D4">
         <v>148</v>
@@ -490,13 +669,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
         <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
       </c>
       <c r="D5">
         <v>170</v>
@@ -504,21 +683,220 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="D6">
         <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>